<commit_message>
fluxo de caixa Connectfibra
</commit_message>
<xml_diff>
--- a/2020/CONTROLE DE CAIXA MAIO 2020/26-05-2020_FluxoDeCaixa.xlsx
+++ b/2020/CONTROLE DE CAIXA MAIO 2020/26-05-2020_FluxoDeCaixa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael_Campos\Documents\GitHub\ConnectFibra\2020\CONTROLE DE CAIXA MAIO 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4469E297-F9CB-4764-87B4-570B6F4BFC95}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6563BF59-92CE-4050-9E0A-9727A1C4557A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caixa de Henrique" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Caixa de Rose" sheetId="2" r:id="rId3"/>
     <sheet name="Relatório do Caixa" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -239,7 +238,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -256,7 +255,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -554,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -875,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1011,9 @@
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4">
+        <v>631</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1053,7 +1054,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="5">
-        <v>43976</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,7 +1138,7 @@
       </c>
       <c r="B13" s="13">
         <f>'Caixa de Deborah'!B19+'Caixa de Henrique'!B17+'Caixa de Rose'!B19</f>
-        <v>1649</v>
+        <v>2280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>